<commit_message>
New sensitivity analysis (delta, SALib) 2
</commit_message>
<xml_diff>
--- a/pyindp/Sensitivity_SALib/Results.xlsx
+++ b/pyindp/Sensitivity_SALib/Results.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="res" sheetId="1" r:id="rId1"/>
     <sheet name="csv" sheetId="2" r:id="rId2"/>
     <sheet name="perf" sheetId="3" r:id="rId3"/>
     <sheet name="csv (2)" sheetId="4" r:id="rId4"/>
+    <sheet name="corr" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'csv (2)'!$A$1:$F$91</definedName>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="708" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="30">
   <si>
     <t>L</t>
   </si>
@@ -95,6 +96,21 @@
   </si>
   <si>
     <t>ScaleFree</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>Perf</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>resource allocation</t>
+  </si>
+  <si>
+    <t>topology</t>
   </si>
 </sst>
 </file>
@@ -905,11 +921,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448379136"/>
-        <c:axId val="448378352"/>
+        <c:axId val="463036232"/>
+        <c:axId val="463029176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448379136"/>
+        <c:axId val="463036232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1008,7 +1024,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448378352"/>
+        <c:crossAx val="463029176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1016,7 +1032,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448378352"/>
+        <c:axId val="463029176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1121,7 +1137,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448379136"/>
+        <c:crossAx val="463036232"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1620,11 +1636,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="448378744"/>
-        <c:axId val="448383056"/>
+        <c:axId val="463029568"/>
+        <c:axId val="463029960"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="448378744"/>
+        <c:axId val="463029568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1723,7 +1739,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448383056"/>
+        <c:crossAx val="463029960"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1731,7 +1747,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="448383056"/>
+        <c:axId val="463029960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1836,7 +1852,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="448378744"/>
+        <c:crossAx val="463029568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2643,11 +2659,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="523266640"/>
-        <c:axId val="523267032"/>
+        <c:axId val="463031136"/>
+        <c:axId val="463031528"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="523266640"/>
+        <c:axId val="463031136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2679,7 +2695,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2746,7 +2761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523267032"/>
+        <c:crossAx val="463031528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2754,7 +2769,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="523267032"/>
+        <c:axId val="463031528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2813,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -2859,7 +2873,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="523266640"/>
+        <c:crossAx val="463031136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3357,11 +3371,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="525608200"/>
-        <c:axId val="525608592"/>
+        <c:axId val="463038584"/>
+        <c:axId val="463032704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="525608200"/>
+        <c:axId val="463038584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3393,7 +3407,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3460,7 +3473,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525608592"/>
+        <c:crossAx val="463032704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3468,7 +3481,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="525608592"/>
+        <c:axId val="463032704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3512,7 +3525,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -3573,7 +3585,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="525608200"/>
+        <c:crossAx val="463038584"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6558,7 +6570,7 @@
   <dimension ref="A1:N32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:Q1048576"/>
+      <selection activeCell="B3" sqref="B3:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10431,15 +10443,15 @@
         <v>8.4587450846298512E-2</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:L32" si="5">_xlfn.RANK.EQ(C4,C$3:C$8)</f>
+        <f t="shared" ref="L4:L8" si="5">_xlfn.RANK.EQ(C4,C$3:C$8)</f>
         <v>5</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" ref="M4:M32" si="6">_xlfn.RANK.EQ(D4,D$3:D$8)</f>
+        <f t="shared" ref="M4:M8" si="6">_xlfn.RANK.EQ(D4,D$3:D$8)</f>
         <v>4</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" ref="N4:N32" si="7">_xlfn.RANK.EQ(E4,E$3:E$8)</f>
+        <f t="shared" ref="N4:N8" si="7">_xlfn.RANK.EQ(E4,E$3:E$8)</f>
         <v>4</v>
       </c>
     </row>
@@ -10731,15 +10743,15 @@
         <v>0.21535742063211483</v>
       </c>
       <c r="L10" s="3">
-        <f t="shared" ref="L10:L32" si="9">_xlfn.RANK.EQ(C10,C$9:C$14)</f>
+        <f t="shared" ref="L10:L14" si="9">_xlfn.RANK.EQ(C10,C$9:C$14)</f>
         <v>6</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" ref="M10:M32" si="10">_xlfn.RANK.EQ(D10,D$9:D$14)</f>
+        <f t="shared" ref="M10:M14" si="10">_xlfn.RANK.EQ(D10,D$9:D$14)</f>
         <v>2</v>
       </c>
       <c r="N10" s="3">
-        <f t="shared" ref="N10:N32" si="11">_xlfn.RANK.EQ(E10,E$9:E$14)</f>
+        <f t="shared" ref="N10:N14" si="11">_xlfn.RANK.EQ(E10,E$9:E$14)</f>
         <v>2</v>
       </c>
     </row>
@@ -11031,15 +11043,15 @@
         <v>0.25560393959184335</v>
       </c>
       <c r="L16" s="3">
-        <f t="shared" ref="L16:L32" si="13">_xlfn.RANK.EQ(C16,C$15:C$20)</f>
+        <f t="shared" ref="L16:L20" si="13">_xlfn.RANK.EQ(C16,C$15:C$20)</f>
         <v>6</v>
       </c>
       <c r="M16" s="3">
-        <f t="shared" ref="M16:M32" si="14">_xlfn.RANK.EQ(D16,D$15:D$20)</f>
+        <f t="shared" ref="M16:M20" si="14">_xlfn.RANK.EQ(D16,D$15:D$20)</f>
         <v>5</v>
       </c>
       <c r="N16" s="3">
-        <f t="shared" ref="N16:N32" si="15">_xlfn.RANK.EQ(E16,E$15:E$20)</f>
+        <f t="shared" ref="N16:N20" si="15">_xlfn.RANK.EQ(E16,E$15:E$20)</f>
         <v>5</v>
       </c>
     </row>
@@ -11331,15 +11343,15 @@
         <v>0.26627307214542173</v>
       </c>
       <c r="L22" s="3">
-        <f t="shared" ref="L22:L32" si="17">_xlfn.RANK.EQ(C22,C$21:C$26)</f>
+        <f t="shared" ref="L22:L26" si="17">_xlfn.RANK.EQ(C22,C$21:C$26)</f>
         <v>6</v>
       </c>
       <c r="M22" s="3">
-        <f t="shared" ref="M22:M32" si="18">_xlfn.RANK.EQ(D22,D$21:D$26)</f>
+        <f t="shared" ref="M22:M26" si="18">_xlfn.RANK.EQ(D22,D$21:D$26)</f>
         <v>5</v>
       </c>
       <c r="N22" s="3">
-        <f t="shared" ref="N22:N32" si="19">_xlfn.RANK.EQ(E22,E$21:E$26)</f>
+        <f t="shared" ref="N22:N26" si="19">_xlfn.RANK.EQ(E22,E$21:E$26)</f>
         <v>4</v>
       </c>
     </row>
@@ -11876,7 +11888,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
@@ -13975,4 +13987,768 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.18544500674188399</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.150624860548596</v>
+      </c>
+      <c r="F2" s="3">
+        <v>-0.46233895137604197</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-3.0034122805841001E-2</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0.31779146242647899</v>
+      </c>
+      <c r="I2" s="3">
+        <v>-0.19155481103006</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.221914027208482</v>
+      </c>
+      <c r="E3" s="3">
+        <v>4.3728973323468097E-2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.19839526989477099</v>
+      </c>
+      <c r="G3" s="3">
+        <v>7.3847382794208896E-2</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0.45977667089902802</v>
+      </c>
+      <c r="I3" s="3">
+        <v>-0.111133021285902</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.26693425196933901</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.11035270683757201</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.10423923225034699</v>
+      </c>
+      <c r="G4" s="3">
+        <v>6.8776664209955804E-2</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0.37162900053199499</v>
+      </c>
+      <c r="I4" s="3">
+        <v>-5.6512639790080602E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.15303952265808099</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.11867790236978901</v>
+      </c>
+      <c r="F5" s="3">
+        <v>-0.44607027505193497</v>
+      </c>
+      <c r="G5" s="3">
+        <v>-4.4808477511574699E-2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0.315973476367443</v>
+      </c>
+      <c r="I5" s="3">
+        <v>-0.204277945709889</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0.148098509965573</v>
+      </c>
+      <c r="E6" s="3">
+        <v>1.41275344698901E-2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0.22034882424265101</v>
+      </c>
+      <c r="G6" s="3">
+        <v>5.8089593808869897E-2</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.468373444593564</v>
+      </c>
+      <c r="I6" s="3">
+        <v>-0.13027552228639699</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.21890138837402801</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.12383859212408101</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.115045739270119</v>
+      </c>
+      <c r="G7" s="3">
+        <v>7.7305818589911104E-2</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.373261092767673</v>
+      </c>
+      <c r="I7" s="3">
+        <v>-3.5082804158082397E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.16625221488539499</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.16870843129226801</v>
+      </c>
+      <c r="F8" s="3">
+        <v>-0.445843406187511</v>
+      </c>
+      <c r="G8" s="3">
+        <v>1.9017845760993499E-2</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.239321879249144</v>
+      </c>
+      <c r="I8" s="3">
+        <v>-0.230746320368067</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.30305914173722098</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.22702726893090699</v>
+      </c>
+      <c r="F9" s="3">
+        <v>0.22907067125195099</v>
+      </c>
+      <c r="G9" s="3">
+        <v>0.22469401728858901</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0.37256901973165202</v>
+      </c>
+      <c r="I9" s="3">
+        <v>-5.7079320957264E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0.24362642893027001</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.15783072142538601</v>
+      </c>
+      <c r="F10" s="3">
+        <v>0.146073122996184</v>
+      </c>
+      <c r="G10" s="3">
+        <v>0.128977469474921</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0.34425934995400298</v>
+      </c>
+      <c r="I10" s="3">
+        <v>-4.8153830415384097E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>25</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>4.09621661299234E-2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.19073042324824499</v>
+      </c>
+      <c r="F11" s="3">
+        <v>-6.8308818078633995E-2</v>
+      </c>
+      <c r="G11" s="3">
+        <v>0.103840689403619</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.20513333956146801</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.73250077812567205</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>0.21121307683905099</v>
+      </c>
+      <c r="E12" s="3">
+        <v>-5.9383175005606498E-2</v>
+      </c>
+      <c r="F12" s="3">
+        <v>-0.24784004399555001</v>
+      </c>
+      <c r="G12" s="3">
+        <v>-0.32592739055657399</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0.19116061462314701</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.72942549399849199</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>-0.15958562009718499</v>
+      </c>
+      <c r="E13" s="3">
+        <v>-2.2278475179336701E-2</v>
+      </c>
+      <c r="F13" s="3">
+        <v>-0.31000886041238301</v>
+      </c>
+      <c r="G13" s="3">
+        <v>0.15163286684494201</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7.6139324628371197E-2</v>
+      </c>
+      <c r="I13" s="3">
+        <v>0.77559517842484904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14">
+        <v>-0.26513962065020802</v>
+      </c>
+      <c r="E14">
+        <v>-0.15923010283262401</v>
+      </c>
+      <c r="F14">
+        <v>0.223246676976282</v>
+      </c>
+      <c r="G14">
+        <v>-0.168607630001915</v>
+      </c>
+      <c r="H14">
+        <v>-0.19856442014405301</v>
+      </c>
+      <c r="I14">
+        <v>0.14304032829397301</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>-0.353168981817856</v>
+      </c>
+      <c r="E15">
+        <v>-0.13956640763703601</v>
+      </c>
+      <c r="F15">
+        <v>-0.22970854383186201</v>
+      </c>
+      <c r="G15">
+        <v>-0.30372253765930601</v>
+      </c>
+      <c r="H15">
+        <v>-0.33581088983651902</v>
+      </c>
+      <c r="I15">
+        <v>5.5657449477409499E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>-0.35548991570254701</v>
+      </c>
+      <c r="E16">
+        <v>-0.22476755429607001</v>
+      </c>
+      <c r="F16">
+        <v>-0.22394034752415001</v>
+      </c>
+      <c r="G16">
+        <v>-0.23128036176090899</v>
+      </c>
+      <c r="H16">
+        <v>-0.24294041363118099</v>
+      </c>
+      <c r="I16">
+        <v>6.2492251716399799E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17">
+        <v>-0.26847409487843998</v>
+      </c>
+      <c r="E17">
+        <v>-0.14325033243643001</v>
+      </c>
+      <c r="F17">
+        <v>0.20936183172769399</v>
+      </c>
+      <c r="G17">
+        <v>-0.159180554883981</v>
+      </c>
+      <c r="H17">
+        <v>-0.20129867521322201</v>
+      </c>
+      <c r="I17">
+        <v>0.170963689394525</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>-0.32104814598054698</v>
+      </c>
+      <c r="E18">
+        <v>-7.0051858042689902E-2</v>
+      </c>
+      <c r="F18">
+        <v>-0.24244893822156699</v>
+      </c>
+      <c r="G18">
+        <v>-0.30344222873061599</v>
+      </c>
+      <c r="H18">
+        <v>-0.37611648859756602</v>
+      </c>
+      <c r="I18">
+        <v>9.0784756925338397E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>-0.34857488502366302</v>
+      </c>
+      <c r="E19">
+        <v>-0.19599446219619299</v>
+      </c>
+      <c r="F19">
+        <v>-0.19645955396751</v>
+      </c>
+      <c r="G19">
+        <v>-0.22815189784673601</v>
+      </c>
+      <c r="H19">
+        <v>-0.25158831045847102</v>
+      </c>
+      <c r="I19">
+        <v>7.98673253800017E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20">
+        <v>-0.24414250318637701</v>
+      </c>
+      <c r="E20">
+        <v>-0.20004937114395599</v>
+      </c>
+      <c r="F20">
+        <v>0.232130685782343</v>
+      </c>
+      <c r="G20">
+        <v>-0.168493138269277</v>
+      </c>
+      <c r="H20">
+        <v>-0.19553404898208299</v>
+      </c>
+      <c r="I20">
+        <v>0.12348814704529899</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>-0.38865437169775602</v>
+      </c>
+      <c r="E21">
+        <v>-0.24878535935782201</v>
+      </c>
+      <c r="F21">
+        <v>-0.28118271027200897</v>
+      </c>
+      <c r="G21">
+        <v>-0.38378971858125099</v>
+      </c>
+      <c r="H21">
+        <v>-0.28865743278669798</v>
+      </c>
+      <c r="I21">
+        <v>1.6890704813190199E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>-0.35052087981552799</v>
+      </c>
+      <c r="E22">
+        <v>-0.23338554484114299</v>
+      </c>
+      <c r="F22">
+        <v>-0.20217274194495299</v>
+      </c>
+      <c r="G22">
+        <v>-0.25586035448232203</v>
+      </c>
+      <c r="H22">
+        <v>-0.219761806034941</v>
+      </c>
+      <c r="I22">
+        <v>8.6466415396621102E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" t="s">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>-0.24323318165542901</v>
+      </c>
+      <c r="E23">
+        <v>-0.151829712110683</v>
+      </c>
+      <c r="F23">
+        <v>0.219403467322069</v>
+      </c>
+      <c r="G23">
+        <v>-8.6502885520220105E-2</v>
+      </c>
+      <c r="H23">
+        <v>-0.14556333879976599</v>
+      </c>
+      <c r="I23">
+        <v>0.213163717961767</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>-0.38809824097108597</v>
+      </c>
+      <c r="E24">
+        <v>-9.6247617369724495E-2</v>
+      </c>
+      <c r="F24">
+        <v>-0.28826110309574299</v>
+      </c>
+      <c r="G24">
+        <v>-0.30001655767400398</v>
+      </c>
+      <c r="H24">
+        <v>-0.34504656856478</v>
+      </c>
+      <c r="I24">
+        <v>8.6725897694696796E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>-0.44343570399427601</v>
+      </c>
+      <c r="E25">
+        <v>-0.202385047512287</v>
+      </c>
+      <c r="F25">
+        <v>-0.24041631426721499</v>
+      </c>
+      <c r="G25">
+        <v>-0.16664540686704801</v>
+      </c>
+      <c r="H25">
+        <v>-0.106754663173869</v>
+      </c>
+      <c r="I25">
+        <v>0.183946908210842</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D2:I13">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D14:I25">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>